<commit_message>
Push before I delete a bunch of stuff from npixfit
</commit_message>
<xml_diff>
--- a/Bundles.xlsx
+++ b/Bundles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36540" yWindow="-440" windowWidth="38400" windowHeight="24000" tabRatio="944" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="36540" windowHeight="23560" tabRatio="944" firstSheet="3" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="212">
   <si>
     <t>More</t>
   </si>
@@ -553,9 +553,6 @@
   </si>
   <si>
     <t>D Slat</t>
-  </si>
-  <si>
-    <t>WHOA WAIT, WE DIDN'T CHARACTERIZE Gs</t>
   </si>
   <si>
     <t>F Slat</t>
@@ -2934,6 +2931,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3110,6 +3108,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -3145,6 +3144,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6414,6 +6414,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6560,6 +6561,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -6595,6 +6597,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -25874,7 +25877,7 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C32" s="322">
         <v>204</v>
@@ -39394,8 +39397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -39834,14 +39837,14 @@
         <v>0.53500000000000003</v>
       </c>
       <c r="F29" s="303">
-        <f>SUM(E29:E37)+9*0.8128</f>
-        <v>12.0952</v>
+        <f>SUM(E29:E37)+9*0.8128 +0.4572</f>
+        <v>12.5524</v>
       </c>
       <c r="G29" s="303">
         <v>12.2</v>
       </c>
       <c r="H29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -39973,7 +39976,7 @@
         <v>12.3</v>
       </c>
       <c r="H38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -55668,10 +55671,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -55707,20 +55710,22 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="87" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="185" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="185"/>
+      <c r="C2" s="185">
+        <v>46</v>
+      </c>
       <c r="D2" s="303"/>
-      <c r="E2" s="306" t="e">
+      <c r="E2" s="306">
         <f>AVERAGE(LOOKUP(C2,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C2,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C2,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C2,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F2" s="185" t="e">
+        <v>0.88</v>
+      </c>
+      <c r="F2" s="185">
         <f>SUM(E2:E8)+7*0.97282</f>
-        <v>#N/A</v>
+        <v>12.969739999999998</v>
       </c>
       <c r="G2" s="185">
         <v>13.19</v>
@@ -55729,10 +55734,12 @@
     <row r="3" spans="1:7">
       <c r="A3" s="87"/>
       <c r="B3" s="185"/>
-      <c r="C3" s="185"/>
-      <c r="E3" s="306" t="e">
+      <c r="C3" s="185">
+        <v>45</v>
+      </c>
+      <c r="E3" s="306">
         <f>AVERAGE(LOOKUP(C3,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C3,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C3,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C3,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.87749999999999995</v>
       </c>
       <c r="F3" s="185"/>
       <c r="G3" s="185"/>
@@ -55740,10 +55747,12 @@
     <row r="4" spans="1:7">
       <c r="A4" s="87"/>
       <c r="B4" s="185"/>
-      <c r="C4" s="185"/>
-      <c r="E4" s="306" t="e">
+      <c r="C4" s="185">
+        <v>44</v>
+      </c>
+      <c r="E4" s="306">
         <f>AVERAGE(LOOKUP(C4,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C4,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C4,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C4,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="F4" s="185"/>
       <c r="G4" s="185"/>
@@ -55751,10 +55760,12 @@
     <row r="5" spans="1:7">
       <c r="A5" s="87"/>
       <c r="B5" s="185"/>
-      <c r="C5" s="185"/>
-      <c r="E5" s="306" t="e">
+      <c r="C5" s="185">
+        <v>43</v>
+      </c>
+      <c r="E5" s="306">
         <f>AVERAGE(LOOKUP(C5,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C5,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C5,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C5,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.875</v>
       </c>
       <c r="F5" s="185"/>
       <c r="G5" s="185"/>
@@ -55762,10 +55773,12 @@
     <row r="6" spans="1:7">
       <c r="A6" s="87"/>
       <c r="B6" s="185"/>
-      <c r="C6" s="185"/>
-      <c r="E6" s="306" t="e">
+      <c r="C6" s="185">
+        <v>42</v>
+      </c>
+      <c r="E6" s="306">
         <f>AVERAGE(LOOKUP(C6,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C6,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C6,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C6,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.90249999999999997</v>
       </c>
       <c r="F6" s="185"/>
       <c r="G6" s="185"/>
@@ -55773,10 +55786,12 @@
     <row r="7" spans="1:7">
       <c r="A7" s="87"/>
       <c r="B7" s="185"/>
-      <c r="C7" s="185"/>
-      <c r="E7" s="306" t="e">
+      <c r="C7" s="185">
+        <v>41</v>
+      </c>
+      <c r="E7" s="306">
         <f>AVERAGE(LOOKUP(C7,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C7,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C7,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C7,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.88</v>
       </c>
       <c r="F7" s="185"/>
       <c r="G7" s="185"/>
@@ -55786,30 +55801,34 @@
       <c r="B8" s="185" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="185"/>
-      <c r="E8" s="306" t="e">
+      <c r="C8" s="185">
+        <v>40</v>
+      </c>
+      <c r="E8" s="314">
         <f>AVERAGE(LOOKUP(C8,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C8,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C8,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C8,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.88</v>
       </c>
       <c r="F8" s="185"/>
       <c r="G8" s="185"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="303" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="303"/>
+      <c r="C9" s="303">
+        <v>54</v>
+      </c>
       <c r="D9" s="303"/>
-      <c r="E9" s="306" t="e">
+      <c r="E9" s="306">
         <f>AVERAGE(LOOKUP(C9,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C9,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C9,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C9,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F9" s="303" t="e">
+        <v>0.875</v>
+      </c>
+      <c r="F9" s="303">
         <f>SUM(E9:E15)+7*0.97282</f>
-        <v>#N/A</v>
+        <v>13.02224</v>
       </c>
       <c r="G9" s="303">
         <v>13.14</v>
@@ -55818,10 +55837,12 @@
     <row r="10" spans="1:7">
       <c r="A10" s="87"/>
       <c r="B10" s="185"/>
-      <c r="C10" s="185"/>
-      <c r="E10" s="306" t="e">
+      <c r="C10" s="185">
+        <v>53</v>
+      </c>
+      <c r="E10" s="306">
         <f>AVERAGE(LOOKUP(C10,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C10,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C10,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C10,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="F10" s="185"/>
       <c r="G10" s="185"/>
@@ -55829,10 +55850,12 @@
     <row r="11" spans="1:7">
       <c r="A11" s="87"/>
       <c r="B11" s="185"/>
-      <c r="C11" s="185"/>
-      <c r="E11" s="306" t="e">
+      <c r="C11" s="185">
+        <v>52</v>
+      </c>
+      <c r="E11" s="306">
         <f>AVERAGE(LOOKUP(C11,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C11,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C11,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C11,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="F11" s="185"/>
       <c r="G11" s="185"/>
@@ -55840,10 +55863,12 @@
     <row r="12" spans="1:7">
       <c r="A12" s="87"/>
       <c r="B12" s="185"/>
-      <c r="C12" s="185"/>
-      <c r="E12" s="306" t="e">
+      <c r="C12" s="185">
+        <v>39</v>
+      </c>
+      <c r="E12" s="306">
         <f>AVERAGE(LOOKUP(C12,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C12,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C12,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C12,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="F12" s="185"/>
       <c r="G12" s="185"/>
@@ -55851,10 +55876,12 @@
     <row r="13" spans="1:7">
       <c r="A13" s="87"/>
       <c r="B13" s="185"/>
-      <c r="C13" s="185"/>
-      <c r="E13" s="306" t="e">
+      <c r="C13" s="185">
+        <v>38</v>
+      </c>
+      <c r="E13" s="306">
         <f>AVERAGE(LOOKUP(C13,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C13,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C13,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C13,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.90750000000000008</v>
       </c>
       <c r="F13" s="185"/>
       <c r="G13" s="185"/>
@@ -55862,10 +55889,12 @@
     <row r="14" spans="1:7">
       <c r="A14" s="87"/>
       <c r="B14" s="185"/>
-      <c r="C14" s="185"/>
-      <c r="E14" s="306" t="e">
+      <c r="C14" s="185">
+        <v>49</v>
+      </c>
+      <c r="E14" s="306">
         <f>AVERAGE(LOOKUP(C14,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C14,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C14,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C14,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="F14" s="185"/>
       <c r="G14" s="185"/>
@@ -55875,19 +55904,16 @@
       <c r="B15" s="253" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="253"/>
+      <c r="C15" s="253">
+        <v>48</v>
+      </c>
       <c r="D15" s="103"/>
-      <c r="E15" s="306" t="e">
+      <c r="E15" s="314">
         <f>AVERAGE(LOOKUP(C15,Es!$A$12:$A$28,Es!$E$12:$E$28),LOOKUP(C15,Es!$A$12:$A$28,Es!$F$12:$F$28),LOOKUP(C15,Es!$A$12:$A$28,Es!$G$12:$G$28),LOOKUP(C15,Es!$A$12:$A$28,Es!$H$12:$H$28))</f>
-        <v>#N/A</v>
+        <v>0.89</v>
       </c>
       <c r="F15" s="253"/>
       <c r="G15" s="253"/>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" t="s">
-        <v>165</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -55924,7 +55950,7 @@
         <v>108</v>
       </c>
       <c r="C1" s="304" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D1" s="309" t="s">
         <v>126</v>
@@ -55941,7 +55967,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="87" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="185" t="s">
         <v>110</v>
@@ -56031,7 +56057,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" s="303" t="s">
         <v>110</v>
@@ -56121,7 +56147,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14" s="303" t="s">
         <v>110</v>
@@ -56211,7 +56237,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B20" s="303" t="s">
         <v>110</v>
@@ -56339,7 +56365,7 @@
         <v>108</v>
       </c>
       <c r="C1" s="304" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D1" s="309" t="s">
         <v>126</v>
@@ -56356,7 +56382,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2" s="185" t="s">
         <v>110</v>
@@ -56446,7 +56472,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8" s="303" t="s">
         <v>110</v>
@@ -56536,7 +56562,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B14" s="303" t="s">
         <v>110</v>
@@ -56664,7 +56690,7 @@
         <v>108</v>
       </c>
       <c r="C1" s="304" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="309" t="s">
         <v>126</v>
@@ -56681,7 +56707,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="87" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" s="185" t="s">
         <v>110</v>
@@ -56758,7 +56784,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="303" t="s">
         <v>110</v>
@@ -56835,7 +56861,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="303" t="s">
         <v>110</v>
@@ -56912,7 +56938,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" s="303" t="s">
         <v>110</v>
@@ -57027,7 +57053,7 @@
         <v>108</v>
       </c>
       <c r="C1" s="304" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D1" s="309" t="s">
         <v>126</v>
@@ -57044,7 +57070,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="87" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2" s="185" t="s">
         <v>110</v>
@@ -57121,7 +57147,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" s="303" t="s">
         <v>110</v>
@@ -57233,7 +57259,7 @@
         <v>108</v>
       </c>
       <c r="C1" s="304" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" s="309" t="s">
         <v>126</v>
@@ -57250,7 +57276,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="87" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2" s="185" t="s">
         <v>110</v>
@@ -57314,7 +57340,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B6" s="303" t="s">
         <v>110</v>
@@ -57378,7 +57404,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" s="303" t="s">
         <v>110</v>
@@ -57442,7 +57468,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B14" s="303" t="s">
         <v>110</v>
@@ -57507,7 +57533,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="302" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18" s="327" t="s">
         <v>110</v>
@@ -57608,7 +57634,7 @@
         <v>108</v>
       </c>
       <c r="C1" s="304" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D1" s="309" t="s">
         <v>126</v>
@@ -57625,7 +57651,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="87" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="185" t="s">
         <v>110</v>
@@ -57676,7 +57702,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5" s="303" t="s">
         <v>110</v>
@@ -57727,7 +57753,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" s="303" t="s">
         <v>110</v>
@@ -57778,7 +57804,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" s="303" t="s">
         <v>110</v>
@@ -57830,7 +57856,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="302" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B14" s="327" t="s">
         <v>110</v>
@@ -57917,7 +57943,7 @@
         <v>108</v>
       </c>
       <c r="C1" s="304" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D1" s="309" t="s">
         <v>126</v>
@@ -57934,7 +57960,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="87" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="185" t="s">
         <v>110</v>
@@ -57972,7 +57998,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" s="303" t="s">
         <v>110</v>
@@ -58010,7 +58036,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" s="303" t="s">
         <v>110</v>
@@ -58048,7 +58074,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B8" s="303" t="s">
         <v>110</v>
@@ -58087,7 +58113,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="302" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10" s="327" t="s">
         <v>110</v>
@@ -58160,7 +58186,7 @@
         <v>108</v>
       </c>
       <c r="C1" s="304" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D1" s="309" t="s">
         <v>126</v>
@@ -58177,7 +58203,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="87" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="185"/>
       <c r="C2" s="185">
@@ -58198,7 +58224,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="303"/>
       <c r="C3" s="303">
@@ -58219,7 +58245,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" s="303"/>
       <c r="C4" s="303">
@@ -58240,7 +58266,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="329" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5" s="328"/>
       <c r="C5" s="328">
@@ -58295,7 +58321,7 @@
         <v>108</v>
       </c>
       <c r="C1" s="304" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D1" s="309" t="s">
         <v>126</v>
@@ -58312,7 +58338,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="329" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="328"/>
       <c r="C2" s="328">
@@ -68654,7 +68680,7 @@
       <c r="Y50" s="35"/>
       <c r="Z50" s="35"/>
       <c r="AA50" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:27">

</xml_diff>